<commit_message>
Update DSA student list
</commit_message>
<xml_diff>
--- a/list-students/DSA (5).xlsx
+++ b/list-students/DSA (5).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\data-structure-and-algorithms\list-students\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BB737D-C9CA-405F-A904-F52EDA3A7F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A72C5E-FE7A-4ABC-9C60-4589F5BA42A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA (5) - Nhom 1" sheetId="2" r:id="rId1"/>
@@ -1451,12 +1451,6 @@
     <xf numFmtId="14" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1489,6 +1483,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1845,10 +1845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,103 +1863,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="6" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2145,51 +2145,51 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2">
-        <v>38671</v>
+        <v>38570</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E18" s="2">
-        <v>38570</v>
+        <v>38656</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -2197,25 +2197,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E19" s="2">
-        <v>38656</v>
+        <v>38593</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2223,10 +2223,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>47</v>
@@ -2235,117 +2235,117 @@
         <v>52</v>
       </c>
       <c r="E20" s="2">
-        <v>38593</v>
+        <v>38514</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E21" s="2">
-        <v>38514</v>
+        <v>38591</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E22" s="2">
-        <v>38591</v>
+        <v>38551</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E23" s="2">
-        <v>38551</v>
+        <v>38308</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E24" s="2">
-        <v>38308</v>
+        <v>38521</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2353,25 +2353,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E25" s="2">
-        <v>38521</v>
+        <v>38360</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -2379,25 +2379,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>79</v>
       </c>
       <c r="E26" s="2">
-        <v>38360</v>
+        <v>38516</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2405,25 +2405,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E27" s="2">
-        <v>38516</v>
+        <v>38445</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -2431,25 +2431,25 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E28" s="2">
-        <v>38445</v>
+        <v>38403</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2457,25 +2457,25 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E29" s="2">
-        <v>38403</v>
+        <v>38503</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -2483,25 +2483,25 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E30" s="2">
-        <v>38503</v>
+        <v>38653</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -2509,25 +2509,25 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E31" s="2">
-        <v>38653</v>
+        <v>38463</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -2535,25 +2535,25 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E32" s="2">
-        <v>38463</v>
+        <v>38629</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -2561,25 +2561,25 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E33" s="2">
-        <v>38629</v>
+        <v>38409</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -2587,25 +2587,25 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E34" s="2">
-        <v>38409</v>
+        <v>38514</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -2613,25 +2613,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E35" s="2">
-        <v>38514</v>
+        <v>38489</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -2639,25 +2639,25 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E36" s="2">
-        <v>38489</v>
+        <v>38484</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -2665,25 +2665,25 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="E37" s="2">
-        <v>38484</v>
+        <v>38692</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -2691,25 +2691,25 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E38" s="2">
-        <v>38692</v>
+        <v>38549</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -2717,25 +2717,25 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E39" s="2">
-        <v>38549</v>
+        <v>38494</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -2743,25 +2743,25 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E40" s="2">
-        <v>38494</v>
+        <v>38534</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -2769,25 +2769,25 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E41" s="2">
-        <v>38534</v>
+        <v>38522</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -2795,58 +2795,38 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E42" s="2">
-        <v>38522</v>
+        <v>38500</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>34</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E43" s="2">
-        <v>38500</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H43">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A7:A9"/>
@@ -2856,12 +2836,6 @@
     <mergeCell ref="C8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2869,10 +2843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0233D4-BFFB-4851-934F-2C3AAC87B0D6}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2883,107 +2857,107 @@
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="6" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -3008,7 +2982,7 @@
         <v>259</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3086,7 +3060,7 @@
         <v>247</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,7 +3216,7 @@
         <v>225</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3476,7 +3450,7 @@
         <v>196</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3606,7 +3580,7 @@
         <v>178</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3684,7 +3658,7 @@
         <v>166</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3814,11 +3788,43 @@
         <v>146</v>
       </c>
       <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="2">
+        <v>38671</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H42">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A7:A9"/>
@@ -3828,12 +3834,6 @@
     <mergeCell ref="C8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>